<commit_message>
Testing for Research Paper
</commit_message>
<xml_diff>
--- a/Models/All Test/OCR Handwritten/Joey's Cafe Handwritten.xlsx
+++ b/Models/All Test/OCR Handwritten/Joey's Cafe Handwritten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KJSCE\LY\Project\Intelligent-Document-Analyzer\Models\All Test\OCR Handwritten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59F25FA-431D-4DE8-95B0-5B95AB80BC49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B48396-3412-4D4D-ADB0-2FF2DB090F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>Service</t>
-  </si>
-  <si>
-    <t>Food Qaulity</t>
   </si>
   <si>
     <t>Would You Recommend Us to a Friend?</t>
@@ -735,6 +732,9 @@
   <si>
     <t>food arrived quickly</t>
   </si>
+  <si>
+    <t>Food Quality</t>
+  </si>
 </sst>
 </file>
 
@@ -1183,7 +1183,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1227,16 +1227,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -1256,37 +1256,37 @@
     </row>
     <row r="2" spans="1:27" ht="13.8">
       <c r="A2" s="27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="7">
         <v>9981170856</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="7">
         <v>24092021</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="K2" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="L2" s="11">
         <v>0</v>
@@ -1313,31 +1313,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="7">
         <v>9384429030</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="7">
         <v>5012020</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="11">
         <v>1</v>
@@ -1364,31 +1364,31 @@
         <v>3</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="7">
         <v>9974976882</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="7">
         <v>23052021</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
@@ -1415,31 +1415,31 @@
         <v>4</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="7">
         <v>9248065776</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="7">
         <v>14012022</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L5" s="11">
         <v>1</v>
@@ -1466,31 +1466,31 @@
         <v>5</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7">
         <v>9197281262</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="7">
         <v>30102020</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K6" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L6" s="11">
         <v>0</v>
@@ -1517,31 +1517,31 @@
         <v>6</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="7">
         <v>9185845649</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F7" s="7">
         <v>15062020</v>
       </c>
       <c r="G7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J7" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
@@ -1568,31 +1568,31 @@
         <v>7</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="7">
         <v>9935519056</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="7">
         <v>26092020</v>
       </c>
       <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L8" s="11">
         <v>1</v>
@@ -1619,31 +1619,31 @@
         <v>8</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="7">
         <v>9901552268</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F9" s="7">
         <v>8062020</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L9" s="11">
         <v>0</v>
@@ -1670,31 +1670,31 @@
         <v>9</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7">
         <v>9738667464</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="7">
         <v>27062020</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="11">
         <v>0</v>
@@ -1721,31 +1721,31 @@
         <v>10</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="7">
         <v>9740840764</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="7">
         <v>16082021</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="11">
         <v>1</v>
@@ -1772,31 +1772,31 @@
         <v>11</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="7">
         <v>9561936700</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" s="7">
         <v>15022021</v>
       </c>
       <c r="G12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J12" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L12" s="11">
         <v>0</v>
@@ -1823,31 +1823,31 @@
         <v>12</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="7">
         <v>9564194282</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="7">
         <v>31012020</v>
       </c>
       <c r="G13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K13" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L13" s="11">
         <v>0</v>
@@ -1874,31 +1874,31 @@
         <v>13</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="7">
         <v>9701822161</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F14" s="7">
         <v>10072021</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L14" s="11">
         <v>0</v>
@@ -1925,31 +1925,31 @@
         <v>14</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D15" s="7">
         <v>9775859962</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="7">
         <v>4042021</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L15" s="11">
         <v>1</v>
@@ -1976,31 +1976,31 @@
         <v>15</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D16" s="7">
         <v>9010033501</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="7">
         <v>15072021</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K16" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L16" s="11">
         <v>0</v>
@@ -2027,31 +2027,31 @@
         <v>16</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="7">
         <v>9904150239</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F17" s="7">
         <v>23042020</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J17" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K17" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L17" s="11">
         <v>1</v>
@@ -2078,31 +2078,31 @@
         <v>17</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D18" s="7">
         <v>9589939394</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F18" s="7">
         <v>14112020</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J18" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18" s="11">
         <v>1</v>
@@ -2129,31 +2129,31 @@
         <v>18</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="7">
         <v>9929219667</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="7">
         <v>8082020</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J19" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L19" s="11">
         <v>1</v>
@@ -2180,31 +2180,31 @@
         <v>19</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="7">
         <v>9108704679</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F20" s="7">
         <v>27092020</v>
       </c>
       <c r="G20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K20" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L20" s="11">
         <v>1</v>
@@ -2231,31 +2231,31 @@
         <v>20</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D21" s="7">
         <v>9775133962</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F21" s="7">
         <v>10032021</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J21" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L21" s="11">
         <v>0</v>
@@ -2282,31 +2282,31 @@
         <v>21</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D22" s="7">
         <v>9042291415</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" s="7">
         <v>1022021</v>
       </c>
       <c r="G22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J22" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="L22" s="11">
         <v>1</v>
@@ -2333,31 +2333,31 @@
         <v>22</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="7">
         <v>9727839801</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F23" s="7">
         <v>20042021</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J23" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K23" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L23" s="11">
         <v>0</v>
@@ -2384,31 +2384,31 @@
         <v>23</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D24" s="7">
         <v>9039608913</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F24" s="7">
         <v>10032020</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K24" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L24" s="11">
         <v>1</v>
@@ -2435,31 +2435,31 @@
         <v>24</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D25" s="7">
         <v>9729246200</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="7">
         <v>23112021</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K25" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L25" s="11">
         <v>0</v>
@@ -2486,31 +2486,31 @@
         <v>25</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D26" s="7">
         <v>9217621011</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F26" s="7">
         <v>30072020</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J26" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K26" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L26" s="11">
         <v>0</v>
@@ -2533,37 +2533,37 @@
     </row>
     <row r="27" spans="1:27" ht="13.8">
       <c r="A27" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="5">
         <v>26</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="7">
         <v>9515393187</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F27" s="7">
         <v>25112020</v>
       </c>
       <c r="G27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="I27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="5" t="s">
+      <c r="J27" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J27" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K27" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L27" s="11">
         <v>0</v>
@@ -2590,31 +2590,31 @@
         <v>27</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="7">
         <v>9543063196</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F28" s="7">
         <v>19112021</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J28" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K28" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L28" s="11">
         <v>1</v>
@@ -2641,31 +2641,31 @@
         <v>28</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="7">
         <v>9914587953</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="7">
         <v>10042021</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J29" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K29" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L29" s="11">
         <v>0</v>
@@ -2692,31 +2692,31 @@
         <v>29</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D30" s="7">
         <v>9621130744</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F30" s="7">
         <v>31122020</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I30" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L30" s="11">
         <v>1</v>
@@ -2743,31 +2743,31 @@
         <v>30</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D31" s="7">
         <v>9566033411</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F31" s="7">
         <v>1092021</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I31" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J31" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="L31" s="11">
         <v>0</v>
@@ -2794,31 +2794,31 @@
         <v>31</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" s="7">
         <v>9690230620</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="7">
         <v>15042020</v>
       </c>
       <c r="G32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="I32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I32" s="5" t="s">
+      <c r="J32" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J32" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K32" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="L32" s="11">
         <v>0</v>
@@ -2845,31 +2845,31 @@
         <v>32</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D33" s="7">
         <v>9143086457</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F33" s="7">
         <v>5042021</v>
       </c>
       <c r="G33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J33" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K33" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L33" s="11">
         <v>1</v>
@@ -2896,31 +2896,31 @@
         <v>33</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="7">
         <v>9548439304</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F34" s="7">
         <v>29032021</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J34" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L34" s="11">
         <v>1</v>
@@ -2947,31 +2947,31 @@
         <v>34</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D35" s="7">
         <v>9415713966</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="7">
         <v>3092021</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J35" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L35" s="11">
         <v>0</v>
@@ -2998,31 +2998,31 @@
         <v>35</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D36" s="7">
         <v>9536084502</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F36" s="7">
         <v>23072021</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J36" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K36" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L36" s="11">
         <v>0</v>
@@ -3049,31 +3049,31 @@
         <v>36</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D37" s="7">
         <v>9227441575</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37" s="7">
         <v>18052021</v>
       </c>
       <c r="G37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="I37" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="J37" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="J37" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K37" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L37" s="11">
         <v>0</v>
@@ -3100,31 +3100,31 @@
         <v>37</v>
       </c>
       <c r="C38" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D38" s="7">
         <v>9734914602</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F38" s="7">
         <v>7062020</v>
       </c>
       <c r="G38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J38" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K38" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L38" s="11">
         <v>0</v>
@@ -3151,31 +3151,31 @@
         <v>38</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D39" s="7">
         <v>9522213128</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F39" s="7">
         <v>6092021</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I39" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J39" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K39" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L39" s="11">
         <v>0</v>
@@ -3202,31 +3202,31 @@
         <v>39</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D40" s="7">
         <v>9773296666</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="7">
         <v>27122020</v>
       </c>
       <c r="G40" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J40" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J40" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K40" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L40" s="11">
         <v>1</v>
@@ -3253,31 +3253,31 @@
         <v>40</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D41" s="7">
         <v>9780826193</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F41" s="7">
         <v>16092020</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J41" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J41" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="K41" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L41" s="11">
         <v>0</v>
@@ -3304,31 +3304,31 @@
         <v>41</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D42" s="7">
         <v>9245081862</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F42" s="7">
         <v>1012020</v>
       </c>
       <c r="G42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H42" s="5" t="s">
+      <c r="I42" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J42" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K42" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L42" s="11">
         <v>1</v>
@@ -3355,31 +3355,31 @@
         <v>42</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D43" s="7">
         <v>9725330703</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F43" s="7">
         <v>24102021</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J43" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L43" s="11">
         <v>0</v>
@@ -3406,31 +3406,31 @@
         <v>43</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D44" s="7">
         <v>9844111573</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F44" s="7">
         <v>27082021</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K44" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="L44" s="11">
         <v>1</v>
@@ -3457,31 +3457,31 @@
         <v>44</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D45" s="7">
         <v>9548951719</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F45" s="7">
         <v>13112020</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I45" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K45" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L45" s="11">
         <v>1</v>
@@ -3508,31 +3508,31 @@
         <v>45</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D46" s="7">
         <v>9114344452</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46" s="7">
         <v>17012020</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I46" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J46" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K46" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L46" s="11">
         <v>1</v>
@@ -3559,31 +3559,31 @@
         <v>46</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D47" s="7">
         <v>9620324375</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F47" s="7">
         <v>9112020</v>
       </c>
       <c r="G47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H47" s="5" t="s">
+      <c r="I47" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I47" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J47" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K47" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L47" s="11">
         <v>0</v>
@@ -3610,31 +3610,31 @@
         <v>47</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D48" s="7">
         <v>9835432117</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" s="7">
         <v>4102020</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I48" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I48" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J48" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K48" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L48" s="11">
         <v>0</v>
@@ -3661,31 +3661,31 @@
         <v>48</v>
       </c>
       <c r="C49" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D49" s="7">
         <v>9001335424</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F49" s="7">
         <v>11012021</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L49" s="11">
         <v>1</v>
@@ -3712,31 +3712,31 @@
         <v>49</v>
       </c>
       <c r="C50" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D50" s="7">
         <v>9764043920</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F50" s="7">
         <v>5102021</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K50" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L50" s="11">
         <v>0</v>
@@ -3763,31 +3763,31 @@
         <v>50</v>
       </c>
       <c r="C51" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D51" s="7">
         <v>9880504483</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F51" s="7">
         <v>12102021</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J51" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K51" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L51" s="11">
         <v>0</v>
@@ -3810,37 +3810,37 @@
     </row>
     <row r="52" spans="1:27" ht="13.8">
       <c r="A52" s="27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B52" s="5">
         <v>51</v>
       </c>
       <c r="C52" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D52" s="7">
         <v>9881757178</v>
       </c>
       <c r="E52" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F52" s="7">
         <v>12032021</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H52" s="5" t="s">
+      <c r="I52" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I52" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J52" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K52" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L52" s="11">
         <v>1</v>
@@ -3867,31 +3867,31 @@
         <v>52</v>
       </c>
       <c r="C53" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D53" s="7">
         <v>9347083459</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F53" s="7">
         <v>7122021</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H53" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I53" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I53" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J53" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K53" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="L53" s="11">
         <v>0</v>
@@ -3918,31 +3918,31 @@
         <v>53</v>
       </c>
       <c r="C54" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D54" s="7">
         <v>9750925074</v>
       </c>
       <c r="E54" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F54" s="7">
         <v>24122021</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K54" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="L54" s="11">
         <v>1</v>
@@ -3969,31 +3969,31 @@
         <v>54</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" s="7">
         <v>9769008457</v>
       </c>
       <c r="E55" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F55" s="7">
         <v>26082021</v>
       </c>
       <c r="G55" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J55" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K55" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L55" s="11">
         <v>1</v>
@@ -4020,31 +4020,31 @@
         <v>55</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D56" s="7">
         <v>9731274483</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F56" s="7">
         <v>25012022</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K56" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L56" s="11">
         <v>0</v>
@@ -4071,31 +4071,31 @@
         <v>56</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D57" s="7">
         <v>9360230068</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F57" s="7">
         <v>4112020</v>
       </c>
       <c r="G57" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H57" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="I57" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I57" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J57" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K57" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L57" s="11">
         <v>1</v>
@@ -4122,31 +4122,31 @@
         <v>57</v>
       </c>
       <c r="C58" s="13" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D58" s="7">
         <v>9983360629</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F58" s="7">
         <v>30012021</v>
       </c>
       <c r="G58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J58" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H58" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J58" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K58" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L58" s="11">
         <v>0</v>
@@ -4173,31 +4173,31 @@
         <v>58</v>
       </c>
       <c r="C59" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D59" s="7">
         <v>9565126764</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F59" s="7">
         <v>11092021</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K59" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L59" s="11">
         <v>1</v>
@@ -4224,31 +4224,31 @@
         <v>59</v>
       </c>
       <c r="C60" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D60" s="7">
         <v>9592327230</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F60" s="7">
         <v>26022020</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K60" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L60" s="11">
         <v>0</v>
@@ -4275,31 +4275,31 @@
         <v>60</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D61" s="7">
         <v>9400649522</v>
       </c>
       <c r="E61" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F61" s="7">
         <v>2112021</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J61" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K61" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L61" s="11">
         <v>1</v>
@@ -4326,31 +4326,31 @@
         <v>61</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D62" s="20">
         <v>9838163323</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F62" s="7">
         <v>16082021</v>
       </c>
       <c r="G62" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H62" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="I62" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I62" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J62" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K62" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L62" s="11">
         <v>0</v>
@@ -4377,31 +4377,31 @@
         <v>62</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D63" s="20">
         <v>9578848391</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F63" s="7">
         <v>15022021</v>
       </c>
       <c r="G63" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J63" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H63" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J63" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K63" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L63" s="11">
         <v>1</v>
@@ -4428,31 +4428,31 @@
         <v>63</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D64" s="20">
         <v>9053736003</v>
       </c>
       <c r="E64" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F64" s="7">
         <v>31012020</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H64" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I64" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K64" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L64" s="11">
         <v>1</v>
@@ -4479,31 +4479,31 @@
         <v>64</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D65" s="20">
         <v>9162522172</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F65" s="7">
         <v>10072021</v>
       </c>
       <c r="G65" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I65" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J65" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K65" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L65" s="11">
         <v>0</v>
@@ -4530,31 +4530,31 @@
         <v>65</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D66" s="20">
         <v>9372367287</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F66" s="7">
         <v>4042021</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I66" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J66" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I66" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J66" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K66" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L66" s="11">
         <v>0</v>
@@ -4581,31 +4581,31 @@
         <v>66</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D67" s="20">
         <v>9426622146</v>
       </c>
       <c r="E67" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F67" s="7">
         <v>15072021</v>
       </c>
       <c r="G67" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H67" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H67" s="5" t="s">
+      <c r="I67" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I67" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J67" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K67" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L67" s="11">
         <v>0</v>
@@ -4632,31 +4632,31 @@
         <v>67</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D68" s="20">
         <v>9096595526</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F68" s="7">
         <v>23042020</v>
       </c>
       <c r="G68" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I68" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J68" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H68" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I68" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J68" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K68" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L68" s="11">
         <v>1</v>
@@ -4683,31 +4683,31 @@
         <v>68</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D69" s="20">
         <v>9671687387</v>
       </c>
       <c r="E69" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F69" s="7">
         <v>14112020</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H69" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I69" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K69" s="10" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L69" s="11">
         <v>0</v>
@@ -4734,31 +4734,31 @@
         <v>69</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D70" s="20">
         <v>9379401509</v>
       </c>
       <c r="E70" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F70" s="7">
         <v>8082020</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H70" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I70" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K70" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L70" s="11">
         <v>1</v>
@@ -4785,31 +4785,31 @@
         <v>70</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D71" s="20">
         <v>9114856316</v>
       </c>
       <c r="E71" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F71" s="7">
         <v>27092020</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J71" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I71" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J71" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K71" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="L71" s="11">
         <v>1</v>
@@ -4836,31 +4836,31 @@
         <v>71</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D72" s="20">
         <v>9753946124</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F72" s="7">
         <v>30012021</v>
       </c>
       <c r="G72" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H72" s="5" t="s">
+      <c r="I72" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I72" s="5" t="s">
+      <c r="J72" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J72" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K72" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L72" s="11">
         <v>1</v>
@@ -4887,31 +4887,31 @@
         <v>72</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D73" s="20">
         <v>9599912784</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F73" s="7">
         <v>11092021</v>
       </c>
       <c r="G73" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I73" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J73" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H73" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I73" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J73" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K73" s="10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L73" s="11">
         <v>0</v>
@@ -4938,31 +4938,31 @@
         <v>73</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D74" s="20">
         <v>9099822098</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F74" s="7">
         <v>26022020</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H74" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I74" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K74" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="L74" s="11">
         <v>1</v>
@@ -4989,31 +4989,31 @@
         <v>74</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D75" s="20">
         <v>9460985154</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F75" s="7">
         <v>2112021</v>
       </c>
       <c r="G75" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I75" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J75" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H75" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I75" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J75" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K75" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L75" s="11">
         <v>1</v>
@@ -5040,31 +5040,31 @@
         <v>75</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D76" s="20">
         <v>9688091155</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F76" s="7">
         <v>16082021</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H76" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I76" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K76" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L76" s="11">
         <v>0</v>
@@ -5087,37 +5087,37 @@
     </row>
     <row r="77" spans="1:27" ht="13.8">
       <c r="A77" s="27" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B77" s="5">
         <v>76</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D77" s="20">
         <v>9692860224</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F77" s="7">
         <v>15022021</v>
       </c>
       <c r="G77" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H77" s="5" t="s">
+      <c r="I77" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I77" s="5" t="s">
+      <c r="J77" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J77" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K77" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="L77" s="11">
         <v>1</v>
@@ -5144,31 +5144,31 @@
         <v>77</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D78" s="20">
         <v>9448754744</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F78" s="7">
         <v>23052021</v>
       </c>
       <c r="G78" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J78" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H78" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I78" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J78" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K78" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L78" s="11">
         <v>0</v>
@@ -5195,31 +5195,31 @@
         <v>78</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D79" s="20">
         <v>9750860647</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F79" s="7">
         <v>14012022</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H79" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I79" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K79" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L79" s="11">
         <v>0</v>
@@ -5246,31 +5246,31 @@
         <v>79</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D80" s="20">
         <v>9618928711</v>
       </c>
       <c r="E80" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F80" s="7">
         <v>30102020</v>
       </c>
       <c r="G80" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J80" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I80" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J80" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K80" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L80" s="11">
         <v>0</v>
@@ -5297,31 +5297,31 @@
         <v>80</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D81" s="20">
         <v>9270157598</v>
       </c>
       <c r="E81" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F81" s="7">
         <v>15062020</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H81" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I81" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J81" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I81" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J81" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K81" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L81" s="11">
         <v>0</v>
@@ -5348,31 +5348,31 @@
         <v>81</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D82" s="20">
         <v>9779147192</v>
       </c>
       <c r="E82" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F82" s="7">
         <v>26092020</v>
       </c>
       <c r="G82" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H82" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H82" s="5" t="s">
+      <c r="I82" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I82" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J82" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K82" s="10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L82" s="11">
         <v>0</v>
@@ -5399,31 +5399,31 @@
         <v>82</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D83" s="20">
         <v>9993600121</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F83" s="7">
         <v>8062020</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H83" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I83" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I83" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J83" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K83" s="10" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L83" s="11">
         <v>0</v>
@@ -5450,31 +5450,31 @@
         <v>83</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D84" s="20">
         <v>9180824708</v>
       </c>
       <c r="E84" s="18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F84" s="7">
         <v>27062020</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H84" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I84" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K84" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="L84" s="11">
         <v>0</v>
@@ -5501,31 +5501,31 @@
         <v>84</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D85" s="20">
         <v>9979617686</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F85" s="7">
         <v>16082021</v>
       </c>
       <c r="G85" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I85" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H85" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J85" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K85" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L85" s="11">
         <v>1</v>
@@ -5552,31 +5552,31 @@
         <v>85</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D86" s="20">
         <v>9562495119</v>
       </c>
       <c r="E86" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F86" s="7">
         <v>15022021</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H86" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I86" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J86" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K86" s="10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L86" s="11">
         <v>0</v>
@@ -5603,31 +5603,31 @@
         <v>86</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D87" s="20">
         <v>9244092577</v>
       </c>
       <c r="E87" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F87" s="7">
         <v>31012020</v>
       </c>
       <c r="G87" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H87" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H87" s="5" t="s">
+      <c r="I87" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I87" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J87" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K87" s="10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="L87" s="11">
         <v>0</v>
@@ -5654,31 +5654,31 @@
         <v>87</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D88" s="20">
         <v>9089186869</v>
       </c>
       <c r="E88" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F88" s="7">
         <v>10072021</v>
       </c>
       <c r="G88" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H88" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J88" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H88" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I88" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J88" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K88" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L88" s="11">
         <v>0</v>
@@ -5705,31 +5705,31 @@
         <v>88</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D89" s="20">
         <v>9904531019</v>
       </c>
       <c r="E89" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F89" s="7">
         <v>27122020</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I89" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K89" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="L89" s="11">
         <v>1</v>
@@ -5756,31 +5756,31 @@
         <v>89</v>
       </c>
       <c r="C90" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D90" s="20">
         <v>9011975107</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F90" s="7">
         <v>16092020</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H90" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K90" s="10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="L90" s="11">
         <v>1</v>
@@ -5807,31 +5807,31 @@
         <v>90</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D91" s="20">
         <v>9439238754</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F91" s="7">
         <v>1012020</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H91" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K91" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="L91" s="11">
         <v>1</v>
@@ -5858,31 +5858,31 @@
         <v>91</v>
       </c>
       <c r="C92" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D92" s="20">
         <v>9407785911</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F92" s="7">
         <v>24102021</v>
       </c>
       <c r="G92" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H92" s="5" t="s">
+      <c r="I92" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I92" s="5" t="s">
+      <c r="J92" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J92" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K92" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="L92" s="11">
         <v>0</v>
@@ -5909,31 +5909,31 @@
         <v>92</v>
       </c>
       <c r="C93" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D93" s="20">
         <v>9162002948</v>
       </c>
       <c r="E93" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F93" s="7">
         <v>27082021</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H93" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I93" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="J93" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K93" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L93" s="11">
         <v>1</v>
@@ -5960,31 +5960,31 @@
         <v>93</v>
       </c>
       <c r="C94" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D94" s="20">
         <v>9337955735</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F94" s="7">
         <v>13112020</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H94" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I94" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J94" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L94" s="11">
         <v>0</v>
@@ -6011,31 +6011,31 @@
         <v>94</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D95" s="20">
         <v>9523102037</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F95" s="7">
         <v>17012020</v>
       </c>
       <c r="G95" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H95" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J95" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H95" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I95" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J95" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K95" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L95" s="11">
         <v>0</v>
@@ -6062,31 +6062,31 @@
         <v>95</v>
       </c>
       <c r="C96" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D96" s="20">
         <v>9763533980</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F96" s="7">
         <v>2112021</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H96" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="L96" s="11">
         <v>0</v>
@@ -6113,31 +6113,31 @@
         <v>96</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D97" s="20">
         <v>9475031069</v>
       </c>
       <c r="E97" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F97" s="7">
         <v>16092020</v>
       </c>
       <c r="G97" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H97" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H97" s="5" t="s">
+      <c r="I97" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I97" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="J97" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="L97" s="11">
         <v>0</v>
@@ -6164,31 +6164,31 @@
         <v>97</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D98" s="20">
         <v>9022148583</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F98" s="7">
         <v>1012020</v>
       </c>
       <c r="G98" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H98" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J98" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H98" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I98" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="J98" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K98" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L98" s="11">
         <v>1</v>
@@ -6215,31 +6215,31 @@
         <v>98</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D99" s="20">
         <v>9246498899</v>
       </c>
       <c r="E99" s="16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F99" s="7">
         <v>24102021</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H99" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I99" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J99" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L99" s="11">
         <v>0</v>
@@ -6266,31 +6266,31 @@
         <v>99</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D100" s="20">
         <v>9942344699</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F100" s="7">
         <v>27082021</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I100" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="L100" s="11">
         <v>1</v>
@@ -6317,31 +6317,31 @@
         <v>100</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D101" s="20">
         <v>9326996530</v>
       </c>
       <c r="E101" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F101" s="7">
         <v>27082021</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H101" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I101" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J101" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I101" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J101" s="9" t="s">
-        <v>18</v>
-      </c>
       <c r="K101" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L101" s="11">
         <v>1</v>

</xml_diff>